<commit_message>
commit 1 ( 25/04/25 )
생산 계획 CRUD, 검색 , 필터, 정렬
제품 관리 > 상품 등록 CRUD
</commit_message>
<xml_diff>
--- a/ProductionPlan.xlsx
+++ b/ProductionPlan.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fileVersion appName="HCell" lastEdited="12.0" lowestEdited="12.0" rupBuild="0.535"/>
+  <x:fileVersion appName="HCell" lastEdited="9.6" lowestEdited="9.6" rupBuild="1.8898"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIT-303\Desktop\down\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="14115" windowHeight="11310"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="11205"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="productionPlan" sheetId="1" r:id="rId4"/>
@@ -19,9 +14,276 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <x:si>
-    <x:t>AVBC123</x:t>
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="139">
+  <x:si>
+    <x:t>PP-25-002</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전기자전거B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전기자전거A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전동킥보드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-026</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-064</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-005</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-006</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-009</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-008</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-007</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-010</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-013</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-011</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-012</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-016</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-015</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-014</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-027</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-028</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-029</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-025</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-033</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-030</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-032</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-031</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-034</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-035</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-036</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-038</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-037</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-039</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-040</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-043</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-042</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-041</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-046</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-044</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-045</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-048</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-047</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-063-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-004</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-027-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-028-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-026-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-029-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-033-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-031-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-030-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-032-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-034-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-035-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-038-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-036-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-037-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-040-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-039-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-044-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-045-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-043-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-042-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-041-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-050-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-051-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-048-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-046-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-049-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-047-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-055-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-052-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-056-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-054-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-053-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-060-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-059-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-061-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-058-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-057-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-062-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전기자전거C</x:t>
   </x:si>
   <x:si>
     <x:t>생산제품명</x:t>
@@ -43,13 +305,139 @@
   </x:si>
   <x:si>
     <x:t>오토바이</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-057</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-058</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-059</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-060</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-061</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-062</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-063</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-049</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-050</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-051</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-052</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-053</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-054</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-056</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-055</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-MC-001-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-025-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-003-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-005-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-002-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-004-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-007-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-008-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-006-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-009-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-010-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-011-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-014-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-015-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-012-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-013-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PP-25-003</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-019-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-018-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-020-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-016-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-017-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-024-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-001-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-022-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-023-A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P-EB-021-A</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="9">
+  <x:fonts count="10">
     <x:font>
       <x:name val="맑은 고딕"/>
       <x:sz val="11"/>
@@ -81,23 +469,76 @@
       <x:color rgb="ff000000"/>
     </x:font>
     <x:font>
-      <x:name val="맑은 고딕"/>
+      <x:name val="돋움"/>
       <x:sz val="11"/>
       <x:color rgb="ff000000"/>
-      <x:b val="1"/>
     </x:font>
-    <x:font>
-      <x:name val="맑은 고딕"/>
-      <x:sz val="13"/>
-      <x:color rgb="ff9d5cbb"/>
-      <x:b val="1"/>
-    </x:font>
-    <x:font>
-      <x:name val="맑은 고딕"/>
-      <x:sz val="11"/>
-      <x:color rgb="ffbfa100"/>
-      <x:b val="1"/>
-    </x:font>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:font hs:extension="1">
+          <x:name val="맑은 고딕"/>
+          <x:sz val="11"/>
+          <x:color rgb="ff000000"/>
+          <x:b val="1"/>
+          <hs:size val="100"/>
+          <hs:ratio val="100"/>
+          <hs:spacing val="0"/>
+          <hs:offset val="0"/>
+        </x:font>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:font>
+          <x:name val="맑은 고딕"/>
+          <x:sz val="11"/>
+          <x:color rgb="ff000000"/>
+          <x:b val="1"/>
+        </x:font>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:font hs:extension="1">
+          <x:name val="맑은 고딕"/>
+          <x:sz val="13"/>
+          <x:color rgb="ff9d5cbb"/>
+          <x:b val="1"/>
+          <hs:size val="100"/>
+          <hs:ratio val="100"/>
+          <hs:spacing val="0"/>
+          <hs:offset val="0"/>
+        </x:font>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:font>
+          <x:name val="맑은 고딕"/>
+          <x:sz val="13"/>
+          <x:color rgb="ff9d5cbb"/>
+          <x:b val="1"/>
+        </x:font>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:font hs:extension="1">
+          <x:name val="맑은 고딕"/>
+          <x:sz val="11"/>
+          <x:color rgb="ffbfa100"/>
+          <x:b val="1"/>
+          <hs:size val="100"/>
+          <hs:ratio val="100"/>
+          <hs:spacing val="0"/>
+          <hs:offset val="0"/>
+        </x:font>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:font>
+          <x:name val="맑은 고딕"/>
+          <x:sz val="11"/>
+          <x:color rgb="ffbfa100"/>
+          <x:b val="1"/>
+        </x:font>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </x:fonts>
   <x:fills count="2">
     <x:fill>
@@ -116,47 +557,73 @@
         <x:color rgb="ff000000"/>
       </x:right>
       <x:top>
-        <x:color auto="1"/>
+        <x:color indexed="64"/>
       </x:top>
       <x:bottom>
         <x:color rgb="ff000000"/>
       </x:bottom>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
+  <x:cellStyleXfs count="15">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="6">
+  <x:cellXfs count="9">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <x:alignment horizontal="general" vertical="bottom"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <x:alignment horizontal="general" vertical="bottom"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <x:alignment horizontal="left" vertical="bottom"/>
     </x:xf>
-    <x:xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <x:xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <x:alignment horizontal="left" vertical="bottom"/>
     </x:xf>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="bottom"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="bottom"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" hs:applyExtension="1">
@@ -170,9 +637,31 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="bottom"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="bottom"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <x:alignment horizontal="general" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom"/>
+    </x:xf>
   </x:cellXfs>
-  <x:cellStyles count="2">
-    <x:cellStyle name="표준" xfId="0" builtinId="0" iLevel="0"/>
+  <x:cellStyles count="1">
+    <x:cellStyle xfId="0" builtinId="0" iLevel="0"/>
   </x:cellStyles>
   <x:dxfs count="12">
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -180,7 +669,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -263,7 +751,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -298,7 +785,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -343,7 +829,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -387,7 +872,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -395,10 +879,10 @@
           </x:font>
           <x:border>
             <x:left>
-              <x:color auto="1"/>
+              <x:color indexed="64"/>
             </x:left>
             <x:right>
-              <x:color auto="1"/>
+              <x:color indexed="64"/>
             </x:right>
             <x:top style="medium">
               <x:color rgb="ff6182d6"/>
@@ -407,10 +891,10 @@
               <x:color rgb="ff6182d6"/>
             </x:bottom>
             <x:vertical>
-              <x:color auto="1"/>
+              <x:color indexed="64"/>
             </x:vertical>
             <x:horizontal>
-              <x:color auto="1"/>
+              <x:color indexed="64"/>
             </x:horizontal>
           </x:border>
         </x:dxf>
@@ -422,10 +906,10 @@
           </x:font>
           <x:border>
             <x:left>
-              <x:color auto="1"/>
+              <x:color indexed="64"/>
             </x:left>
             <x:right>
-              <x:color auto="1"/>
+              <x:color indexed="64"/>
             </x:right>
             <x:top style="medium">
               <x:color rgb="ff6182d6"/>
@@ -434,10 +918,10 @@
               <x:color rgb="ff6182d6"/>
             </x:bottom>
             <x:vertical>
-              <x:color auto="1"/>
+              <x:color indexed="64"/>
             </x:vertical>
             <x:horizontal>
-              <x:color auto="1"/>
+              <x:color indexed="64"/>
             </x:horizontal>
           </x:border>
         </x:dxf>
@@ -472,7 +956,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -493,7 +976,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -524,7 +1006,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -578,7 +1059,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" name="">
   <a:themeElements>
     <a:clrScheme name="">
       <a:dk1>
@@ -890,13 +1371,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet1"/>
-  <x:dimension ref="A1:AK2"/>
+  <x:dimension ref="A1:AK65"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D11" activeCellId="0" sqref="D11:D11"/>
+    <x:sheetView tabSelected="1" topLeftCell="A41" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="G62" activeCellId="0" sqref="G62:G62"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.39999999999999857891"/>
+  <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
   <x:cols>
     <x:col min="1" max="1" width="14.375" customWidth="1"/>
     <x:col min="2" max="2" width="13" customWidth="1"/>
@@ -909,22 +1390,22 @@
   <x:sheetData>
     <x:row r="1" spans="1:37" ht="19.25">
       <x:c r="A1" s="1" t="s">
-        <x:v>5</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="B1" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="C1" s="1" t="s">
-        <x:v>1</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="D1" s="1" t="s">
-        <x:v>2</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="E1" s="1" t="s">
-        <x:v>3</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F1" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G1" s="4"/>
       <x:c r="H1" s="4"/>
@@ -959,14 +1440,14 @@
       <x:c r="AK1" s="4"/>
     </x:row>
     <x:row r="2" spans="1:37">
-      <x:c r="A2" s="2">
-        <x:v>555555</x:v>
+      <x:c r="A2" s="2" t="s">
+        <x:v>88</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
-        <x:v>0</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>7</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="D2" s="3">
         <x:v>42065</x:v>
@@ -1009,8 +1490,1268 @@
       <x:c r="AJ2" s="5"/>
       <x:c r="AK2" s="5"/>
     </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B3" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="C3" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D3" s="6">
+        <x:v>45748</x:v>
+      </x:c>
+      <x:c r="E3" s="6">
+        <x:v>45777</x:v>
+      </x:c>
+      <x:c r="F3">
+        <x:v>100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B4" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="C4" s="7" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D4" s="8">
+        <x:v>45748</x:v>
+      </x:c>
+      <x:c r="E4" s="8">
+        <x:v>45777</x:v>
+      </x:c>
+      <x:c r="F4" s="7">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B5" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="C5" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D5" s="8">
+        <x:v>45748</x:v>
+      </x:c>
+      <x:c r="E5" s="8">
+        <x:v>45777</x:v>
+      </x:c>
+      <x:c r="F5" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B6" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="C6" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D6" s="8">
+        <x:v>45749</x:v>
+      </x:c>
+      <x:c r="E6" s="8">
+        <x:v>45778</x:v>
+      </x:c>
+      <x:c r="F6" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B7" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="C7" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D7" s="8">
+        <x:v>45750</x:v>
+      </x:c>
+      <x:c r="E7" s="8">
+        <x:v>45779</x:v>
+      </x:c>
+      <x:c r="F7" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="A8" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B8" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="C8" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D8" s="8">
+        <x:v>45751</x:v>
+      </x:c>
+      <x:c r="E8" s="8">
+        <x:v>45780</x:v>
+      </x:c>
+      <x:c r="F8" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="A9" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B9" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="C9" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D9" s="8">
+        <x:v>45752</x:v>
+      </x:c>
+      <x:c r="E9" s="8">
+        <x:v>45781</x:v>
+      </x:c>
+      <x:c r="F9" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="A10" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B10" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="C10" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D10" s="8">
+        <x:v>45753</x:v>
+      </x:c>
+      <x:c r="E10" s="8">
+        <x:v>45782</x:v>
+      </x:c>
+      <x:c r="F10" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B11" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="C11" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D11" s="8">
+        <x:v>45754</x:v>
+      </x:c>
+      <x:c r="E11" s="8">
+        <x:v>45783</x:v>
+      </x:c>
+      <x:c r="F11" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="A12" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B12" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="C12" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D12" s="8">
+        <x:v>45755</x:v>
+      </x:c>
+      <x:c r="E12" s="8">
+        <x:v>45784</x:v>
+      </x:c>
+      <x:c r="F12" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="A13" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B13" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="C13" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D13" s="8">
+        <x:v>45756</x:v>
+      </x:c>
+      <x:c r="E13" s="8">
+        <x:v>45785</x:v>
+      </x:c>
+      <x:c r="F13" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="A14" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B14" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="C14" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D14" s="8">
+        <x:v>45757</x:v>
+      </x:c>
+      <x:c r="E14" s="8">
+        <x:v>45786</x:v>
+      </x:c>
+      <x:c r="F14" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="A15" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B15" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="C15" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D15" s="8">
+        <x:v>45758</x:v>
+      </x:c>
+      <x:c r="E15" s="8">
+        <x:v>45787</x:v>
+      </x:c>
+      <x:c r="F15" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="A16" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B16" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="C16" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D16" s="8">
+        <x:v>45759</x:v>
+      </x:c>
+      <x:c r="E16" s="8">
+        <x:v>45788</x:v>
+      </x:c>
+      <x:c r="F16" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="A17" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B17" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="C17" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D17" s="8">
+        <x:v>45760</x:v>
+      </x:c>
+      <x:c r="E17" s="8">
+        <x:v>45789</x:v>
+      </x:c>
+      <x:c r="F17" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="A18" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B18" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="C18" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D18" s="8">
+        <x:v>45761</x:v>
+      </x:c>
+      <x:c r="E18" s="8">
+        <x:v>45790</x:v>
+      </x:c>
+      <x:c r="F18" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="A19" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B19" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="C19" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D19" s="8">
+        <x:v>45762</x:v>
+      </x:c>
+      <x:c r="E19" s="8">
+        <x:v>45791</x:v>
+      </x:c>
+      <x:c r="F19" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="A20" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B20" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="C20" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D20" s="8">
+        <x:v>45763</x:v>
+      </x:c>
+      <x:c r="E20" s="8">
+        <x:v>45792</x:v>
+      </x:c>
+      <x:c r="F20" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="A21" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B21" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="C21" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D21" s="8">
+        <x:v>45764</x:v>
+      </x:c>
+      <x:c r="E21" s="8">
+        <x:v>45793</x:v>
+      </x:c>
+      <x:c r="F21" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="A22" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B22" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="C22" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D22" s="8">
+        <x:v>45765</x:v>
+      </x:c>
+      <x:c r="E22" s="8">
+        <x:v>45794</x:v>
+      </x:c>
+      <x:c r="F22" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="A23" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B23" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="C23" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D23" s="8">
+        <x:v>45766</x:v>
+      </x:c>
+      <x:c r="E23" s="8">
+        <x:v>45795</x:v>
+      </x:c>
+      <x:c r="F23" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="A24" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B24" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="C24" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D24" s="8">
+        <x:v>45767</x:v>
+      </x:c>
+      <x:c r="E24" s="8">
+        <x:v>45796</x:v>
+      </x:c>
+      <x:c r="F24" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6">
+      <x:c r="A25" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B25" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="C25" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D25" s="8">
+        <x:v>45768</x:v>
+      </x:c>
+      <x:c r="E25" s="8">
+        <x:v>45797</x:v>
+      </x:c>
+      <x:c r="F25" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="A26" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B26" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="C26" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D26" s="8">
+        <x:v>45769</x:v>
+      </x:c>
+      <x:c r="E26" s="8">
+        <x:v>45798</x:v>
+      </x:c>
+      <x:c r="F26" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="A27" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B27" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="C27" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D27" s="8">
+        <x:v>45770</x:v>
+      </x:c>
+      <x:c r="E27" s="8">
+        <x:v>45799</x:v>
+      </x:c>
+      <x:c r="F27" s="7">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="A28" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B28" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="C28" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D28" s="8">
+        <x:v>45771</x:v>
+      </x:c>
+      <x:c r="E28" s="8">
+        <x:v>45800</x:v>
+      </x:c>
+      <x:c r="F28" s="7">
+        <x:v>71</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="A29" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B29" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="C29" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D29" s="8">
+        <x:v>45772</x:v>
+      </x:c>
+      <x:c r="E29" s="8">
+        <x:v>45801</x:v>
+      </x:c>
+      <x:c r="F29" s="7">
+        <x:v>72</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="A30" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B30" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C30" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D30" s="8">
+        <x:v>45773</x:v>
+      </x:c>
+      <x:c r="E30" s="8">
+        <x:v>45802</x:v>
+      </x:c>
+      <x:c r="F30" s="7">
+        <x:v>73</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="A31" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B31" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C31" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D31" s="8">
+        <x:v>45774</x:v>
+      </x:c>
+      <x:c r="E31" s="8">
+        <x:v>45803</x:v>
+      </x:c>
+      <x:c r="F31" s="7">
+        <x:v>74</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="A32" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B32" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C32" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D32" s="8">
+        <x:v>45775</x:v>
+      </x:c>
+      <x:c r="E32" s="8">
+        <x:v>45804</x:v>
+      </x:c>
+      <x:c r="F32" s="7">
+        <x:v>75</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="A33" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B33" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C33" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D33" s="8">
+        <x:v>45776</x:v>
+      </x:c>
+      <x:c r="E33" s="8">
+        <x:v>45805</x:v>
+      </x:c>
+      <x:c r="F33" s="7">
+        <x:v>76</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="A34" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B34" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C34" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D34" s="8">
+        <x:v>45777</x:v>
+      </x:c>
+      <x:c r="E34" s="8">
+        <x:v>45806</x:v>
+      </x:c>
+      <x:c r="F34" s="7">
+        <x:v>77</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="A35" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B35" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="C35" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D35" s="8">
+        <x:v>45778</x:v>
+      </x:c>
+      <x:c r="E35" s="8">
+        <x:v>45807</x:v>
+      </x:c>
+      <x:c r="F35" s="7">
+        <x:v>78</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="A36" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B36" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C36" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D36" s="8">
+        <x:v>45779</x:v>
+      </x:c>
+      <x:c r="E36" s="8">
+        <x:v>45808</x:v>
+      </x:c>
+      <x:c r="F36" s="7">
+        <x:v>79</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="A37" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B37" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C37" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D37" s="8">
+        <x:v>45780</x:v>
+      </x:c>
+      <x:c r="E37" s="8">
+        <x:v>45809</x:v>
+      </x:c>
+      <x:c r="F37" s="7">
+        <x:v>80</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="A38" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B38" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C38" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D38" s="8">
+        <x:v>45781</x:v>
+      </x:c>
+      <x:c r="E38" s="8">
+        <x:v>45810</x:v>
+      </x:c>
+      <x:c r="F38" s="7">
+        <x:v>81</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="A39" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B39" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C39" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D39" s="8">
+        <x:v>45782</x:v>
+      </x:c>
+      <x:c r="E39" s="8">
+        <x:v>45811</x:v>
+      </x:c>
+      <x:c r="F39" s="7">
+        <x:v>82</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6">
+      <x:c r="A40" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B40" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C40" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D40" s="8">
+        <x:v>45783</x:v>
+      </x:c>
+      <x:c r="E40" s="8">
+        <x:v>45812</x:v>
+      </x:c>
+      <x:c r="F40" s="7">
+        <x:v>83</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6">
+      <x:c r="A41" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B41" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="C41" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D41" s="8">
+        <x:v>45784</x:v>
+      </x:c>
+      <x:c r="E41" s="8">
+        <x:v>45813</x:v>
+      </x:c>
+      <x:c r="F41" s="7">
+        <x:v>84</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:6">
+      <x:c r="A42" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B42" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C42" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D42" s="8">
+        <x:v>45785</x:v>
+      </x:c>
+      <x:c r="E42" s="8">
+        <x:v>45814</x:v>
+      </x:c>
+      <x:c r="F42" s="7">
+        <x:v>85</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:6">
+      <x:c r="A43" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B43" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C43" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D43" s="8">
+        <x:v>45786</x:v>
+      </x:c>
+      <x:c r="E43" s="8">
+        <x:v>45815</x:v>
+      </x:c>
+      <x:c r="F43" s="7">
+        <x:v>86</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:6">
+      <x:c r="A44" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B44" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C44" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D44" s="8">
+        <x:v>45787</x:v>
+      </x:c>
+      <x:c r="E44" s="8">
+        <x:v>45816</x:v>
+      </x:c>
+      <x:c r="F44" s="7">
+        <x:v>87</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:6">
+      <x:c r="A45" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B45" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C45" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D45" s="8">
+        <x:v>45788</x:v>
+      </x:c>
+      <x:c r="E45" s="8">
+        <x:v>45817</x:v>
+      </x:c>
+      <x:c r="F45" s="7">
+        <x:v>88</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:6">
+      <x:c r="A46" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B46" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="C46" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D46" s="8">
+        <x:v>45789</x:v>
+      </x:c>
+      <x:c r="E46" s="8">
+        <x:v>45818</x:v>
+      </x:c>
+      <x:c r="F46" s="7">
+        <x:v>89</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:6">
+      <x:c r="A47" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B47" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C47" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D47" s="8">
+        <x:v>45790</x:v>
+      </x:c>
+      <x:c r="E47" s="8">
+        <x:v>45819</x:v>
+      </x:c>
+      <x:c r="F47" s="7">
+        <x:v>90</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:6">
+      <x:c r="A48" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B48" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="C48" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D48" s="8">
+        <x:v>45791</x:v>
+      </x:c>
+      <x:c r="E48" s="8">
+        <x:v>45820</x:v>
+      </x:c>
+      <x:c r="F48" s="7">
+        <x:v>91</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:6">
+      <x:c r="A49" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B49" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="C49" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D49" s="8">
+        <x:v>45792</x:v>
+      </x:c>
+      <x:c r="E49" s="8">
+        <x:v>45821</x:v>
+      </x:c>
+      <x:c r="F49" s="7">
+        <x:v>92</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:6">
+      <x:c r="A50" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B50" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C50" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D50" s="8">
+        <x:v>45793</x:v>
+      </x:c>
+      <x:c r="E50" s="8">
+        <x:v>45822</x:v>
+      </x:c>
+      <x:c r="F50" s="7">
+        <x:v>93</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:6">
+      <x:c r="A51" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="B51" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C51" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D51" s="8">
+        <x:v>45794</x:v>
+      </x:c>
+      <x:c r="E51" s="8">
+        <x:v>45823</x:v>
+      </x:c>
+      <x:c r="F51" s="7">
+        <x:v>94</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:6">
+      <x:c r="A52" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="B52" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="C52" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D52" s="8">
+        <x:v>45795</x:v>
+      </x:c>
+      <x:c r="E52" s="8">
+        <x:v>45824</x:v>
+      </x:c>
+      <x:c r="F52" s="7">
+        <x:v>95</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:6">
+      <x:c r="A53" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="B53" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C53" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D53" s="8">
+        <x:v>45796</x:v>
+      </x:c>
+      <x:c r="E53" s="8">
+        <x:v>45825</x:v>
+      </x:c>
+      <x:c r="F53" s="7">
+        <x:v>96</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:6">
+      <x:c r="A54" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B54" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="C54" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D54" s="8">
+        <x:v>45797</x:v>
+      </x:c>
+      <x:c r="E54" s="8">
+        <x:v>45826</x:v>
+      </x:c>
+      <x:c r="F54" s="7">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:6">
+      <x:c r="A55" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B55" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="C55" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D55" s="8">
+        <x:v>45798</x:v>
+      </x:c>
+      <x:c r="E55" s="8">
+        <x:v>45827</x:v>
+      </x:c>
+      <x:c r="F55" s="7">
+        <x:v>98</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:6">
+      <x:c r="A56" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="B56" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="C56" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D56" s="8">
+        <x:v>45799</x:v>
+      </x:c>
+      <x:c r="E56" s="8">
+        <x:v>45828</x:v>
+      </x:c>
+      <x:c r="F56" s="7">
+        <x:v>99</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:6">
+      <x:c r="A57" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B57" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="C57" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D57" s="8">
+        <x:v>45800</x:v>
+      </x:c>
+      <x:c r="E57" s="8">
+        <x:v>45829</x:v>
+      </x:c>
+      <x:c r="F57" s="7">
+        <x:v>100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:6">
+      <x:c r="A58" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="B58" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="C58" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D58" s="8">
+        <x:v>45801</x:v>
+      </x:c>
+      <x:c r="E58" s="8">
+        <x:v>45830</x:v>
+      </x:c>
+      <x:c r="F58" s="7">
+        <x:v>101</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:6">
+      <x:c r="A59" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B59" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C59" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D59" s="8">
+        <x:v>45802</x:v>
+      </x:c>
+      <x:c r="E59" s="8">
+        <x:v>45831</x:v>
+      </x:c>
+      <x:c r="F59" s="7">
+        <x:v>102</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:6">
+      <x:c r="A60" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="B60" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="C60" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D60" s="8">
+        <x:v>45803</x:v>
+      </x:c>
+      <x:c r="E60" s="8">
+        <x:v>45832</x:v>
+      </x:c>
+      <x:c r="F60" s="7">
+        <x:v>103</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:6">
+      <x:c r="A61" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B61" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="C61" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D61" s="8">
+        <x:v>45804</x:v>
+      </x:c>
+      <x:c r="E61" s="8">
+        <x:v>45833</x:v>
+      </x:c>
+      <x:c r="F61" s="7">
+        <x:v>104</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:6">
+      <x:c r="A62" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="B62" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="C62" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D62" s="8">
+        <x:v>45805</x:v>
+      </x:c>
+      <x:c r="E62" s="8">
+        <x:v>45834</x:v>
+      </x:c>
+      <x:c r="F62" s="7">
+        <x:v>105</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:6">
+      <x:c r="A63" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B63" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="C63" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D63" s="8">
+        <x:v>45806</x:v>
+      </x:c>
+      <x:c r="E63" s="8">
+        <x:v>45835</x:v>
+      </x:c>
+      <x:c r="F63" s="7">
+        <x:v>106</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:6">
+      <x:c r="A64" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="B64" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="C64" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D64" s="8">
+        <x:v>45807</x:v>
+      </x:c>
+      <x:c r="E64" s="8">
+        <x:v>45836</x:v>
+      </x:c>
+      <x:c r="F64" s="7">
+        <x:v>107</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:6">
+      <x:c r="A65" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B65" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C65" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="D65" s="8">
+        <x:v>45808</x:v>
+      </x:c>
+      <x:c r="E65" s="8">
+        <x:v>45837</x:v>
+      </x:c>
+      <x:c r="F65" s="7">
+        <x:v>108</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:pageMargins left="0.69972223043441772461" right="0.69972223043441772461" top="0.75" bottom="0.75" header="0.30000001192092895508" footer="0.30000001192092895508"/>
+  <x:pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>